<commit_message>
added steps.txt and tested the script again
</commit_message>
<xml_diff>
--- a/internship.xlsx
+++ b/internship.xlsx
@@ -3901,7 +3901,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>898 applicants</t>
+          <t>899 applicants</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -6124,7 +6124,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>43 applicants</t>
+          <t>45 applicants</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">

</xml_diff>